<commit_message>
Added: - functional document - Tales scripts.
</commit_message>
<xml_diff>
--- a/Scripts/CR/CR_script.xlsx
+++ b/Scripts/CR/CR_script.xlsx
@@ -53,33 +53,12 @@
     <t>CONTEXTO</t>
   </si>
   <si>
-    <t>PG 01</t>
-  </si>
-  <si>
-    <t>PG 02</t>
-  </si>
-  <si>
-    <t>PG 03</t>
-  </si>
-  <si>
     <t>ILUSTRACIÓN 2</t>
   </si>
   <si>
-    <t>PG 04</t>
-  </si>
-  <si>
-    <t>PG 05</t>
-  </si>
-  <si>
     <t>ILUSTRACIÓN 3</t>
   </si>
   <si>
-    <t>PG 06</t>
-  </si>
-  <si>
-    <t>PG 07</t>
-  </si>
-  <si>
     <t>DISFRAZ</t>
   </si>
   <si>
@@ -137,51 +116,12 @@
     <t>ILUSTRACIÓN 5</t>
   </si>
   <si>
-    <t>PG 08</t>
-  </si>
-  <si>
-    <t>PG 09</t>
-  </si>
-  <si>
-    <t>PG 10</t>
-  </si>
-  <si>
-    <t>PG 11</t>
-  </si>
-  <si>
-    <t>PG 12</t>
-  </si>
-  <si>
-    <t>PG 13</t>
-  </si>
-  <si>
-    <t>PG 14</t>
-  </si>
-  <si>
-    <t>PG 15</t>
-  </si>
-  <si>
-    <t>PG 16</t>
-  </si>
-  <si>
-    <t>PG 17</t>
-  </si>
-  <si>
-    <t>PG 18</t>
-  </si>
-  <si>
     <t>ILUSTRACIÓN 4</t>
   </si>
   <si>
     <t>Bosque</t>
   </si>
   <si>
-    <t>PG 20</t>
-  </si>
-  <si>
-    <t>PG 21</t>
-  </si>
-  <si>
     <t>LOBO</t>
   </si>
   <si>
@@ -274,12 +214,6 @@
     <t>Interior casa de la Abuelita</t>
   </si>
   <si>
-    <t>PG 22</t>
-  </si>
-  <si>
-    <t>PG 23</t>
-  </si>
-  <si>
     <t>CAPERUCITA ROJA, LOBO, ABUELITA, CAZADOR</t>
   </si>
   <si>
@@ -640,6 +574,283 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>LOBO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> está muy gordo porque se ha comido a la abuela y se está poniendo su ropa mientras se mira en el espejo.</t>
+    </r>
+  </si>
+  <si>
+    <t>Un bonito día, Caperucita Roja caminaba tranquilamente por el bosque. Como siempre, llevaba puestas su capa y su caperuza rojas.</t>
+  </si>
+  <si>
+    <t>Mientras atravesaba el bosque, un lobo se plantó delante de ella y le preguntó: «¿Adónde vas, Caperucita?».</t>
+  </si>
+  <si>
+    <t>«¿Y por qué vas con tanta prisa? ¡Mira a tu alrededor! El bosque está lleno de flores y hace un día estupendo», dijo el lobo.</t>
+  </si>
+  <si>
+    <t>«No te salgas del camino y no te distraigas; ve derecha a casa de la abuela», le había dicho su madre antes de salir.</t>
+  </si>
+  <si>
+    <t>«Jejeje. Ha dejado la puerta abierta porque esperaba a Caperucita», pensó el lobo mientras se colaba dentro.</t>
+  </si>
+  <si>
+    <t>… y llegó antes que nadie a casa de la abuelita. ¡Qué listo era!</t>
+  </si>
+  <si>
+    <t>Cuando Caperucita se acercó a la cama algo le olió a chamusquina. «Abuelita», dijo, «¡qué orejas tan grandes tienes!».</t>
+  </si>
+  <si>
+    <t>«Son para oírte mejor», dijo el lobo disfrazado. «¡Y qué ojos más grandes tienes!», siguió Caperucita. «¡Son para verte mejor!».</t>
+  </si>
+  <si>
+    <t>«¡Y tu boca es enorme!», dijo al fin la pobre niña. Entonces el lobo abrió bien la boca y gritó: «¡Es para comerte mejor!».</t>
+  </si>
+  <si>
+    <t>ILUSTRACIÓN 7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Se divide en dos viñetas. En la primera,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CAPERUCITA ROJA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se asoma a la cama de su Abuelita, que en realidad es el </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LOBO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> disfrazado. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAPERUCITA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lo mira con curiosidad. En la segunda, el </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LOBO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se lanza hacia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAPERUCITA ROJA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con la boca abierta.</t>
+    </r>
+  </si>
+  <si>
+    <t>ILUSTRACIÓN 8</t>
+  </si>
+  <si>
+    <t>No muy lejos de allí pasaba un cazador, que se sorprendió mucho al ver la puerta de la casa abierta de par en par.</t>
+  </si>
+  <si>
+    <t>Una vez dentro de la casa, el cazador se encontró con el lobo medio dormido después de la comilona...</t>
+  </si>
+  <si>
+    <t>Gracias al cazador, la niña y su abuelita no se convirtieron en el almuerzo del lobo.</t>
+  </si>
+  <si>
+    <t>«Nunca más me va a engañar un lobo, abuelita», gritó Caperucita. «¡Cómo me alegro de que hayas venido!», le dijo su abuela.</t>
+  </si>
+  <si>
+    <t>Caperucita se quedó pensando en lo que le dijo el lobo: «Seguro que las flores ayudarán a la abuelita a ponerse bien».</t>
+  </si>
+  <si>
+    <t>Pero tuvo cuidado de no comerse su ropa también. ¿Para qué? ¡Para disfrazarse con ella y engañar a Caperucita!</t>
+  </si>
+  <si>
+    <t>«La puerta está abierta… ¡Qué raro!», pensó antes de entrar.</t>
+  </si>
+  <si>
+    <t>«Hummm... Esto es muy raro.», pensó. Y decidió que entraría para ver qué pasaba.</t>
+  </si>
+  <si>
+    <t>Además tenía una cesta llena de fruta para llevársela a su abuela, que estaba enferma.</t>
+  </si>
+  <si>
+    <t>«Voy a la casa de mi abuelita para llevarle fruta porque no se encuentra bien», le contestó la niña.</t>
+  </si>
+  <si>
+    <t>Un rato después, la niña llegó con su cestita que ahora tenía flores además de fruta.</t>
+  </si>
+  <si>
+    <t>idText01</t>
+  </si>
+  <si>
+    <t>idText02</t>
+  </si>
+  <si>
+    <t>idText03</t>
+  </si>
+  <si>
+    <t>idText04</t>
+  </si>
+  <si>
+    <t>idText05</t>
+  </si>
+  <si>
+    <t>idText06</t>
+  </si>
+  <si>
+    <t>idText07</t>
+  </si>
+  <si>
+    <t>idText08</t>
+  </si>
+  <si>
+    <t>idText09</t>
+  </si>
+  <si>
+    <t>idText10</t>
+  </si>
+  <si>
+    <t>idText11</t>
+  </si>
+  <si>
+    <t>idText12</t>
+  </si>
+  <si>
+    <t>idText13</t>
+  </si>
+  <si>
+    <t>idText14</t>
+  </si>
+  <si>
+    <t>idText15</t>
+  </si>
+  <si>
+    <t>idText16</t>
+  </si>
+  <si>
+    <t>idText17</t>
+  </si>
+  <si>
+    <t>idText18</t>
+  </si>
+  <si>
+    <t>idText19</t>
+  </si>
+  <si>
+    <t>idText20</t>
+  </si>
+  <si>
+    <t>idText21</t>
+  </si>
+  <si>
+    <t>idText22</t>
+  </si>
+  <si>
+    <t>idText23</t>
+  </si>
+  <si>
+    <t>Y se entretuvo recogiendo unas pocas flores, sin darse cuenta de que el lobo, en silencio, siguió por el camino…</t>
+  </si>
+  <si>
+    <t>Así fue que el lobo se comió a la abuelita, que estaba en su cama, sin que la pobre se diera cuenta.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>CAZADOR</t>
     </r>
     <r>
@@ -669,222 +880,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>para</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>sacar de ahí a Caperucita y a la abuela.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">El </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LOBO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> está muy gordo porque se ha comido a la abuela y se está poniendo su ropa mientras se mira en el espejo.</t>
-    </r>
-  </si>
-  <si>
-    <t>Un bonito día, Caperucita Roja caminaba tranquilamente por el bosque. Como siempre, llevaba puestas su capa y su caperuza rojas.</t>
-  </si>
-  <si>
-    <t>Mientras atravesaba el bosque, un lobo se plantó delante de ella y le preguntó: «¿Adónde vas, Caperucita?».</t>
-  </si>
-  <si>
-    <t>«¿Y por qué vas con tanta prisa? ¡Mira a tu alrededor! El bosque está lleno de flores y hace un día estupendo», dijo el lobo.</t>
-  </si>
-  <si>
-    <t>«No te salgas del camino y no te distraigas; ve derecha a casa de la abuela», le había dicho su madre antes de salir.</t>
-  </si>
-  <si>
-    <t>«Jejeje. Ha dejado la puerta abierta porque esperaba a Caperucita», pensó el lobo mientras se colaba dentro.</t>
-  </si>
-  <si>
-    <t>… y llegó antes que nadie a casa de la abuelita. ¡Qué listo era!</t>
-  </si>
-  <si>
-    <t>Así fue que el lobo se comió a la abuelita que estaba en su cama sin que la pobre se diera cuenta.</t>
-  </si>
-  <si>
-    <t>Cuando Caperucita se acercó a la cama algo le olió a chamusquina. «Abuelita», dijo, «¡qué orejas tan grandes tienes!».</t>
-  </si>
-  <si>
-    <t>«Son para oírte mejor», dijo el lobo disfrazado. «¡Y qué ojos más grandes tienes!», siguió Caperucita. «¡Son para verte mejor!».</t>
-  </si>
-  <si>
-    <t>«¡Y tu boca es enorme!», dijo al fin la pobre niña. Entonces el lobo abrió bien la boca y gritó: «¡Es para comerte mejor!».</t>
-  </si>
-  <si>
-    <t>ILUSTRACIÓN 7</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Se divide en dos viñetas. En la primera,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CAPERUCITA ROJA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se asoma a la cama de su Abuelita, que en realidad es el </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LOBO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> disfrazado. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CAPERUCITA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lo mira con curiosidad. En la segunda, el </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LOBO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se lanza hacia </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CAPERUCITA ROJA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> con la boca abierta.</t>
-    </r>
-  </si>
-  <si>
-    <t>ILUSTRACIÓN 8</t>
-  </si>
-  <si>
-    <t>PG 19</t>
-  </si>
-  <si>
-    <t>No muy lejos de allí pasaba un cazador, que se sorprendió mucho al ver la puerta de la casa abierta de par en par.</t>
-  </si>
-  <si>
-    <t>… y decidió que aquello no podía ser. «¡Ahora mismo voy a sacar a quienes te has comido otra vez para afuera!»</t>
-  </si>
-  <si>
-    <t>Una vez dentro de la casa, el cazador se encontró con el lobo medio dormido después de la comilona...</t>
-  </si>
-  <si>
-    <t>Gracias al cazador, la niña y su abuelita no se convirtieron en el almuerzo del lobo.</t>
-  </si>
-  <si>
-    <t>«Nunca más me va a engañar un lobo, abuelita», gritó Caperucita. «¡Cómo me alegro de que hayas venido!», le dijo su abuela.</t>
-  </si>
-  <si>
-    <t>Caperucita se quedó pensando en lo que le dijo el lobo: «Seguro que las flores ayudarán a la abuelita a ponerse bien».</t>
-  </si>
-  <si>
-    <t>Y se entretuvo recogiendo unas pocas flores, sin darse cuenta de que el lobo, silencioso, se fue por el camino...</t>
-  </si>
-  <si>
-    <t>Pero tuvo cuidado de no comerse su ropa también. ¿Para qué? ¡Para disfrazarse con ella y engañar a Caperucita!</t>
-  </si>
-  <si>
-    <t>«La puerta está abierta… ¡Qué raro!», pensó antes de entrar.</t>
-  </si>
-  <si>
-    <t>«Hummm... Esto es muy raro.», pensó. Y decidió que entraría para ver qué pasaba.</t>
-  </si>
-  <si>
-    <t>Además tenía una cesta llena de fruta para llevársela a su abuela, que estaba enferma.</t>
-  </si>
-  <si>
-    <t>«Voy a la casa de mi abuelita para llevarle fruta porque no se encuentra bien», le contestó la niña.</t>
-  </si>
-  <si>
-    <t>Un rato después, la niña llegó con su cestita que ahora tenía flores además de fruta.</t>
+    <t>… y decidió que aquello no podía ser. «¡Vamos a ver lo que te has comido, lobo glotón!».</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1256,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1266,17 +1284,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1586,8 +1605,8 @@
   </sheetPr>
   <dimension ref="B1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,115 +1624,115 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="46">
         <v>10</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
       <c r="F3" s="21"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="48">
         <v>23</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
+      <c r="C5" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
+      <c r="C8" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="18"/>
@@ -1722,71 +1741,71 @@
       <c r="F13" s="19"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="B14" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
+      <c r="C15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
+      <c r="C16" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="18"/>
@@ -1796,58 +1815,58 @@
       <c r="F20" s="18"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="39"/>
+      <c r="B21" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="20"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
+      <c r="C22" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
+      <c r="C23" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E25" s="34"/>
       <c r="F25" s="18"/>
@@ -1859,58 +1878,58 @@
       <c r="E26" s="30"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="B27" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="C28" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
+      <c r="C29" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="18"/>
@@ -1919,58 +1938,58 @@
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="42"/>
+      <c r="B33" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
+      <c r="C34" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
+      <c r="C35" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="36"/>
+      <c r="E35" s="37"/>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="18"/>
@@ -1979,58 +1998,58 @@
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
+      <c r="B39" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
       <c r="F39" s="20"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="37"/>
-      <c r="E40" s="38"/>
+      <c r="C40" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="36"/>
+      <c r="E40" s="37"/>
       <c r="F40" s="18"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
+      <c r="C41" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="36"/>
+      <c r="E41" s="37"/>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E42" s="34"/>
       <c r="F42" s="18"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="18"/>
@@ -2039,71 +2058,71 @@
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
+      <c r="B45" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
       <c r="F45" s="20"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="38"/>
+      <c r="C46" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
       <c r="F46" s="18"/>
     </row>
     <row r="47" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D47" s="37"/>
-      <c r="E47" s="38"/>
+      <c r="C47" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="36"/>
+      <c r="E47" s="37"/>
       <c r="F47" s="18"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E48" s="34"/>
       <c r="F48" s="18"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="18"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="18"/>
@@ -2112,54 +2131,54 @@
       <c r="F51" s="18"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
+      <c r="B52" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
+      <c r="C53" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="36"/>
+      <c r="E53" s="37"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
+      <c r="C54" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="36"/>
+      <c r="E54" s="37"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E55" s="26"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E56" s="8"/>
     </row>
@@ -2170,132 +2189,111 @@
       <c r="E57" s="32"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="42"/>
+      <c r="B58" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="41"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D59" s="37"/>
-      <c r="E59" s="38"/>
+      <c r="C59" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D59" s="36"/>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="37"/>
-      <c r="E60" s="38"/>
+      <c r="C60" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="36"/>
+      <c r="E60" s="37"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E62" s="8"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="42"/>
+      <c r="B64" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="41"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="37"/>
-      <c r="E65" s="38"/>
+      <c r="C65" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="36"/>
+      <c r="E65" s="37"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="37"/>
-      <c r="E66" s="38"/>
+      <c r="C66" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E67" s="8"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C66:E66"/>
     <mergeCell ref="B52:E52"/>
@@ -2310,6 +2308,27 @@
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="C60:E60"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait" r:id="rId1"/>
@@ -2338,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2346,7 +2365,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -2354,105 +2373,105 @@
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="53"/>
+      <c r="C6" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="53"/>
+      <c r="C8" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="53"/>
+      <c r="C10" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="53"/>
+      <c r="C12" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="53"/>
+      <c r="C14" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="53"/>
+      <c r="C16" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
-      <c r="C6" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
-      <c r="C8" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="51"/>
-      <c r="C10" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
-      <c r="C12" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="50" t="s">
+      <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="13" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -2464,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2472,7 +2491,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -2480,49 +2499,49 @@
         <v>5</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="s">
-        <v>25</v>
+      <c r="B23" s="52" t="s">
+        <v>18</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="13" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
-        <v>26</v>
+      <c r="B25" s="52" t="s">
+        <v>19</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="51"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="13" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
-        <v>27</v>
+      <c r="B27" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="13" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -2534,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2542,7 +2561,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -2550,105 +2569,105 @@
         <v>5</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="50" t="s">
-        <v>25</v>
+      <c r="B33" s="52" t="s">
+        <v>18</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="51"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="13" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="53"/>
+      <c r="C36" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="51"/>
-      <c r="C36" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="50" t="s">
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="53"/>
+      <c r="C38" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="51"/>
-      <c r="C38" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="51"/>
+      <c r="B40" s="53"/>
       <c r="C40" s="13" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="50" t="s">
-        <v>29</v>
+      <c r="B41" s="52" t="s">
+        <v>22</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="51"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="13" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="51"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="13" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="51"/>
+      <c r="B46" s="53"/>
       <c r="C46" s="13" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -2660,7 +2679,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -2668,7 +2687,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -2676,49 +2695,49 @@
         <v>5</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="50" t="s">
-        <v>25</v>
+      <c r="B51" s="52" t="s">
+        <v>18</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="51"/>
+      <c r="B52" s="53"/>
       <c r="C52" s="13" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="50" t="s">
-        <v>26</v>
+      <c r="B53" s="52" t="s">
+        <v>19</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="51"/>
+      <c r="B54" s="53"/>
       <c r="C54" s="13" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="50" t="s">
-        <v>27</v>
+      <c r="B55" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="51"/>
+      <c r="B56" s="53"/>
       <c r="C56" s="13" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -2730,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
@@ -2740,16 +2759,16 @@
       <c r="C59" s="10"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="53"/>
+      <c r="B60" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="51"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="53"/>
+      <c r="B61" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="51"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C62" s="5"/>
@@ -2759,7 +2778,7 @@
         <v>9</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
@@ -2769,16 +2788,16 @@
       <c r="C64" s="10"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" s="53"/>
+      <c r="B65" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="51"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" s="53"/>
+      <c r="B66" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="51"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="5"/>
@@ -2788,6 +2807,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B60:C60"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
@@ -2804,14 +2831,6 @@
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B60:C60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B60:C60" r:id="rId1" display="Ref. 1"/>

</xml_diff>